<commit_message>
Add sng link to xlsx file
</commit_message>
<xml_diff>
--- a/resources/sheets/Stiletti_downloads_table.xlsx
+++ b/resources/sheets/Stiletti_downloads_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darren/Desktop/dystonia_snRNAseq_2024/resources/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C2D8C8-6F10-224E-8BBA-0645BD9FFA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C52CEC-1AC8-354F-99B9-E8EEF7C85D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="4180" windowWidth="27640" windowHeight="16940" xr2:uid="{644B4AD4-4710-0B4C-A88C-995C077659EC}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$111</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="248">
   <si>
     <t>Basal nuclei (BN) - Body of the Caudate - CaB</t>
   </si>
@@ -780,6 +780,9 @@
   </si>
   <si>
     <t>3ca52ee2-8e5a-4d3f-8165-3458337d59a4</t>
+  </si>
+  <si>
+    <t>fd4b7829-283f-4906-8dc4-7846731894e9</t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882BA3EB-7A5C-FE45-9FBD-B664966EB783}">
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1175,6 +1178,7 @@
     <col min="1" max="1" width="74.5" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1773,7 +1777,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>47</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>93</v>
       </c>
@@ -1789,7 +1793,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -1797,7 +1801,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>97</v>
       </c>
@@ -1805,7 +1809,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
@@ -1813,7 +1817,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>100</v>
       </c>
@@ -1821,7 +1825,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>105</v>
       </c>
@@ -1829,7 +1833,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>36</v>
       </c>
@@ -1837,7 +1841,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>51</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>46</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>91</v>
       </c>
@@ -1869,15 +1873,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>27</v>
       </c>
@@ -1885,7 +1892,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>16</v>
       </c>
@@ -1893,7 +1900,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>99</v>
       </c>

</xml_diff>